<commit_message>
Updated the edit form of Transfer Evalution
</commit_message>
<xml_diff>
--- a/data/transfer_by_CommArts_history.xlsx
+++ b/data/transfer_by_CommArts_history.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="166">
   <si>
     <t xml:space="preserve">State Name</t>
   </si>
@@ -266,202 +266,205 @@
     <t xml:space="preserve">Course was previously numbered HU 8117; received confirmation from MCC faculty that it is equivalent to COM 123</t>
   </si>
   <si>
+    <t xml:space="preserve">White Mountains Community College</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARTS 120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Graphic Design Theory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CA 552</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Graphic Design I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pathway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMM 101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMM 115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduction to Media Writing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CA 500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Media Writing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMM 120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CA 540</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern Essex Community College</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COM 115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduction to Mass Communication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COM 111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Institution Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Course #</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNHM Course #</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNHM Course Title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expires </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Great Bay Community College</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUS 110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduction to Business</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUS 400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIS 112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduction to Object-Oriented Programming</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIS 113</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database Design and Management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIS 148</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduction to Java Programming</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMP 425</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computing Fundamentals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIS 177</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Python</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIS 210</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Structures with Elementary Algorithms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMP 520</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database Design and Development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATA 210</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elements of Data Science</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATA 557</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduction to Data Science and Analytics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATA 220</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Analysis w/R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATA 225</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analytics Capstone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENGL 215</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Writing Technical Documents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENGL 502</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Technical Writing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATH 230</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculus I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATH 425</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATH 235</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Statistics for Engineers and Scientists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMP 490</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Statistics in Computing and Engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATH 245</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linear Algebra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATH 545 OR MATH 645</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduction to Linear Algebra OR Linear Algebra for Applications</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATH 250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculus II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATH 426</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nashua Community College</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARTS 120</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Graphic Design Theory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CA 552</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Graphic Design I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pathway</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMM 101</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMM 115</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Introduction to Media Writing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CA 500</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Media Writing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMM 120</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CA 540</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Northern Essex Community College</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COM 115</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Introduction to Mass Communication</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COM 111</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Institution Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Course #</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNHM Course #</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNHM Course Title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expires </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Great Bay Community College</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BUS 110</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Introduction to Business</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BUS 400</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CIS 112</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Introduction to Object-Oriented Programming</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CIS 113</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Database Design and Management</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CIS 148</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Introduction to Java Programming</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMP 425</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Computing Fundamentals</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CIS 177</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Python</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CIS 210</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data Structures with Elementary Algorithms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMP 520</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Database Design and Development</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DATA 210</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elements of Data Science</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DATA 557</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Introduction to Data Science and Analytics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DATA 220</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data Analysis w/R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DATA 225</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Analytics Capstone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENGL 215</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Writing Technical Documents</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENGL 502</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Technical Writing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MATH 230</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calculus I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MATH 425</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MATH 235</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Statistics for Engineers and Scientists</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMP 490</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Statistics in Computing and Engineering</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MATH 245</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Linear Algebra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MATH 545 OR MATH 645</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Introduction to Linear Algebra OR Linear Algebra for Applications</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MATH 250</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calculus II</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MATH 426</t>
   </si>
   <si>
     <t xml:space="preserve">BUS 101</t>
@@ -681,7 +684,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -731,6 +734,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -790,7 +797,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1287,7 +1294,7 @@
       <c r="A17" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="13" t="s">
         <v>75</v>
       </c>
       <c r="C17" s="6" t="s">
@@ -1306,7 +1313,7 @@
         <v>79</v>
       </c>
       <c r="H17" s="12"/>
-      <c r="I17" s="13" t="s">
+      <c r="I17" s="14" t="s">
         <v>80</v>
       </c>
       <c r="J17" s="12"/>
@@ -1316,7 +1323,7 @@
       <c r="A18" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="13" t="s">
         <v>75</v>
       </c>
       <c r="C18" s="6" t="s">
@@ -1335,7 +1342,7 @@
         <v>39</v>
       </c>
       <c r="H18" s="12"/>
-      <c r="I18" s="13" t="s">
+      <c r="I18" s="14" t="s">
         <v>80</v>
       </c>
       <c r="J18" s="12"/>
@@ -1345,7 +1352,7 @@
       <c r="A19" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="13" t="s">
         <v>75</v>
       </c>
       <c r="C19" s="6" t="s">
@@ -1364,7 +1371,7 @@
         <v>85</v>
       </c>
       <c r="H19" s="12"/>
-      <c r="I19" s="13" t="s">
+      <c r="I19" s="14" t="s">
         <v>80</v>
       </c>
       <c r="J19" s="12"/>
@@ -1374,7 +1381,7 @@
       <c r="A20" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="13" t="s">
         <v>75</v>
       </c>
       <c r="C20" s="6" t="s">
@@ -1393,7 +1400,7 @@
         <v>27</v>
       </c>
       <c r="H20" s="12"/>
-      <c r="I20" s="13" t="s">
+      <c r="I20" s="14" t="s">
         <v>80</v>
       </c>
       <c r="J20" s="12"/>
@@ -1476,7 +1483,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="1" sqref="I20 I3"/>
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1496,67 +1503,67 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="15" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="13" t="s">
+      <c r="A2" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="E2" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="13" t="s">
+      <c r="E2" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="J2" s="13"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="J2" s="14"/>
       <c r="K2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1569,24 +1576,24 @@
       <c r="C3" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="19" t="s">
         <v>23</v>
       </c>
       <c r="H3" s="6"/>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="14" t="s">
         <v>80</v>
       </c>
       <c r="J3" s="6"/>
-      <c r="K3" s="20"/>
+      <c r="K3" s="21"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
@@ -1598,24 +1605,24 @@
       <c r="C4" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="20" t="s">
         <v>23</v>
       </c>
       <c r="H4" s="6"/>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="14" t="s">
         <v>80</v>
       </c>
       <c r="J4" s="6"/>
-      <c r="K4" s="20"/>
+      <c r="K4" s="21"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
@@ -1627,20 +1634,20 @@
       <c r="C5" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="19" t="s">
         <v>15</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="20" t="s">
         <v>108</v>
       </c>
       <c r="H5" s="6"/>
-      <c r="I5" s="13" t="s">
+      <c r="I5" s="14" t="s">
         <v>80</v>
       </c>
       <c r="J5" s="6"/>
@@ -1656,20 +1663,20 @@
       <c r="C6" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="20" t="s">
         <v>23</v>
       </c>
       <c r="H6" s="6"/>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="14" t="s">
         <v>80</v>
       </c>
       <c r="J6" s="6"/>
@@ -1685,20 +1692,20 @@
       <c r="C7" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="19" t="s">
         <v>15</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="19" t="s">
         <v>114</v>
       </c>
       <c r="H7" s="6"/>
-      <c r="I7" s="13" t="s">
+      <c r="I7" s="14" t="s">
         <v>80</v>
       </c>
       <c r="J7" s="6"/>
@@ -1714,20 +1721,20 @@
       <c r="C8" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="19" t="s">
         <v>15</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="G8" s="19" t="s">
         <v>118</v>
       </c>
       <c r="H8" s="6"/>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="14" t="s">
         <v>80</v>
       </c>
       <c r="J8" s="6"/>
@@ -1743,20 +1750,20 @@
       <c r="C9" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="18" t="s">
+      <c r="G9" s="19" t="s">
         <v>23</v>
       </c>
       <c r="H9" s="6"/>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="14" t="s">
         <v>80</v>
       </c>
       <c r="J9" s="6"/>
@@ -1772,20 +1779,20 @@
       <c r="C10" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F10" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="20" t="s">
         <v>23</v>
       </c>
       <c r="H10" s="6"/>
-      <c r="I10" s="13" t="s">
+      <c r="I10" s="14" t="s">
         <v>80</v>
       </c>
       <c r="J10" s="6"/>
@@ -1801,20 +1808,20 @@
       <c r="C11" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="19" t="s">
         <v>15</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="G11" s="19" t="s">
+      <c r="G11" s="20" t="s">
         <v>126</v>
       </c>
       <c r="H11" s="6"/>
-      <c r="I11" s="13" t="s">
+      <c r="I11" s="14" t="s">
         <v>80</v>
       </c>
       <c r="J11" s="6"/>
@@ -1830,20 +1837,20 @@
       <c r="C12" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="19" t="s">
         <v>15</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="G12" s="18" t="s">
+      <c r="G12" s="19" t="s">
         <v>128</v>
       </c>
       <c r="H12" s="6"/>
-      <c r="I12" s="13" t="s">
+      <c r="I12" s="14" t="s">
         <v>80</v>
       </c>
       <c r="J12" s="6"/>
@@ -1859,20 +1866,20 @@
       <c r="C13" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="19" t="s">
         <v>15</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="G13" s="19" t="s">
+      <c r="G13" s="20" t="s">
         <v>133</v>
       </c>
       <c r="H13" s="6"/>
-      <c r="I13" s="13" t="s">
+      <c r="I13" s="14" t="s">
         <v>80</v>
       </c>
       <c r="J13" s="6"/>
@@ -1888,20 +1895,20 @@
       <c r="C14" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="19" t="s">
         <v>15</v>
       </c>
       <c r="F14" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="G14" s="21" t="s">
+      <c r="G14" s="22" t="s">
         <v>137</v>
       </c>
       <c r="H14" s="6"/>
-      <c r="I14" s="13" t="s">
+      <c r="I14" s="14" t="s">
         <v>80</v>
       </c>
       <c r="J14" s="6"/>
@@ -1917,20 +1924,20 @@
       <c r="C15" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="19" t="s">
         <v>15</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="G15" s="18" t="s">
+      <c r="G15" s="19" t="s">
         <v>139</v>
       </c>
       <c r="H15" s="6"/>
-      <c r="I15" s="13" t="s">
+      <c r="I15" s="14" t="s">
         <v>80</v>
       </c>
       <c r="J15" s="6"/>
@@ -1941,25 +1948,25 @@
         <v>57</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>75</v>
+        <v>141</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="D16" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="E16" s="18" t="s">
+      <c r="D16" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="E16" s="19" t="s">
         <v>15</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="G16" s="19" t="s">
+      <c r="G16" s="20" t="s">
         <v>99</v>
       </c>
       <c r="H16" s="6"/>
-      <c r="I16" s="13" t="s">
+      <c r="I16" s="14" t="s">
         <v>80</v>
       </c>
       <c r="J16" s="6"/>
@@ -1970,25 +1977,25 @@
         <v>57</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>75</v>
+        <v>141</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="D17" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="D17" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="E17" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F17" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G17" s="19" t="s">
+      <c r="G17" s="20" t="s">
         <v>23</v>
       </c>
       <c r="H17" s="6"/>
-      <c r="I17" s="13" t="s">
+      <c r="I17" s="14" t="s">
         <v>80</v>
       </c>
       <c r="J17" s="6"/>
@@ -1999,54 +2006,54 @@
         <v>57</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>75</v>
+        <v>141</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="D18" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="E18" s="18" t="s">
+      <c r="D18" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="E18" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F18" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G18" s="19" t="s">
+      <c r="G18" s="20" t="s">
         <v>23</v>
       </c>
       <c r="H18" s="6"/>
-      <c r="I18" s="13" t="s">
+      <c r="I18" s="14" t="s">
         <v>80</v>
       </c>
       <c r="J18" s="6"/>
-      <c r="K18" s="20"/>
+      <c r="K18" s="21"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
         <v>57</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>75</v>
+        <v>141</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="D19" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="D19" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="E19" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F19" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G19" s="19" t="s">
+      <c r="G19" s="20" t="s">
         <v>23</v>
       </c>
       <c r="H19" s="6"/>
-      <c r="I19" s="13" t="s">
+      <c r="I19" s="14" t="s">
         <v>80</v>
       </c>
       <c r="J19" s="6"/>
@@ -2057,25 +2064,25 @@
         <v>57</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>75</v>
+        <v>141</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="D20" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="D20" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="E20" s="19" t="s">
         <v>15</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G20" s="18" t="s">
+      <c r="G20" s="19" t="s">
         <v>108</v>
       </c>
       <c r="H20" s="6"/>
-      <c r="I20" s="13" t="s">
+      <c r="I20" s="14" t="s">
         <v>80</v>
       </c>
       <c r="J20" s="6"/>
@@ -2086,112 +2093,112 @@
         <v>57</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>75</v>
+        <v>141</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="D21" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="E21" s="18" t="s">
+      <c r="D21" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="E21" s="19" t="s">
         <v>15</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="G21" s="19" t="s">
-        <v>152</v>
+      <c r="G21" s="20" t="s">
+        <v>153</v>
       </c>
       <c r="H21" s="6"/>
-      <c r="I21" s="13" t="s">
+      <c r="I21" s="14" t="s">
         <v>80</v>
       </c>
       <c r="J21" s="6"/>
-      <c r="K21" s="20"/>
+      <c r="K21" s="21"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
         <v>57</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>75</v>
+        <v>141</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="D22" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="E22" s="18" t="s">
+      <c r="D22" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="E22" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F22" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G22" s="19" t="s">
+      <c r="G22" s="20" t="s">
         <v>23</v>
       </c>
       <c r="H22" s="6"/>
-      <c r="I22" s="13" t="s">
+      <c r="I22" s="14" t="s">
         <v>80</v>
       </c>
       <c r="J22" s="6"/>
-      <c r="K22" s="20"/>
+      <c r="K22" s="21"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
         <v>57</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>75</v>
+        <v>141</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="D23" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="E23" s="18" t="s">
+      <c r="D23" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="E23" s="19" t="s">
         <v>15</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="G23" s="19" t="s">
         <v>158</v>
       </c>
+      <c r="G23" s="20" t="s">
+        <v>159</v>
+      </c>
       <c r="H23" s="6"/>
-      <c r="I23" s="13" t="s">
+      <c r="I23" s="14" t="s">
         <v>80</v>
       </c>
       <c r="J23" s="6"/>
-      <c r="K23" s="20"/>
+      <c r="K23" s="21"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
         <v>57</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>75</v>
+        <v>141</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="D24" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="D24" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="E24" s="18" t="s">
+      <c r="E24" s="19" t="s">
         <v>15</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="G24" s="19" t="s">
+      <c r="G24" s="20" t="s">
         <v>126</v>
       </c>
       <c r="H24" s="6"/>
-      <c r="I24" s="13" t="s">
+      <c r="I24" s="14" t="s">
         <v>80</v>
       </c>
       <c r="J24" s="6"/>
@@ -2202,54 +2209,54 @@
         <v>57</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>75</v>
+        <v>141</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="D25" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="E25" s="18" t="s">
+      <c r="D25" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="E25" s="19" t="s">
         <v>15</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="G25" s="19" t="s">
+      <c r="G25" s="20" t="s">
         <v>133</v>
       </c>
       <c r="H25" s="6"/>
-      <c r="I25" s="13" t="s">
+      <c r="I25" s="14" t="s">
         <v>80</v>
       </c>
       <c r="J25" s="6"/>
-      <c r="K25" s="20"/>
+      <c r="K25" s="21"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
         <v>57</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>75</v>
+        <v>141</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="D26" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="D26" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="E26" s="18" t="s">
+      <c r="E26" s="19" t="s">
         <v>15</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="G26" s="18" t="s">
+      <c r="G26" s="19" t="s">
         <v>128</v>
       </c>
       <c r="H26" s="6"/>
-      <c r="I26" s="13" t="s">
+      <c r="I26" s="14" t="s">
         <v>80</v>
       </c>
       <c r="J26" s="6"/>
@@ -2260,25 +2267,25 @@
         <v>57</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>75</v>
+        <v>141</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="D27" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="D27" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="E27" s="18" t="s">
+      <c r="E27" s="19" t="s">
         <v>15</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="G27" s="19" t="s">
+      <c r="G27" s="20" t="s">
         <v>139</v>
       </c>
       <c r="H27" s="6"/>
-      <c r="I27" s="13" t="s">
+      <c r="I27" s="14" t="s">
         <v>80</v>
       </c>
       <c r="J27" s="6"/>
@@ -2289,25 +2296,25 @@
         <v>57</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>75</v>
+        <v>141</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="D28" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="D28" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="E28" s="18" t="s">
+      <c r="E28" s="19" t="s">
         <v>15</v>
       </c>
       <c r="F28" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="G28" s="21" t="s">
+      <c r="G28" s="22" t="s">
         <v>137</v>
       </c>
       <c r="H28" s="6"/>
-      <c r="I28" s="13" t="s">
+      <c r="I28" s="14" t="s">
         <v>80</v>
       </c>
       <c r="J28" s="6"/>

</xml_diff>